<commit_message>
Find salary using pre keywords
</commit_message>
<xml_diff>
--- a/non_code/benefits_truth.xlsx
+++ b/non_code/benefits_truth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/workspaces/tasks_across_space/non_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAF05CA-CCC3-1648-8309-0551A5F325FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE13C7C-CC08-584A-A245-DA9FC125C569}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{9CCDBE04-1331-2A40-9C3A-F2E5E74B60BB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9CCDBE04-1331-2A40-9C3A-F2E5E74B60BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Salary info is tracked
</commit_message>
<xml_diff>
--- a/non_code/benefits_truth.xlsx
+++ b/non_code/benefits_truth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/workspaces/tasks_across_space/non_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE13C7C-CC08-584A-A245-DA9FC125C569}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4424263-D6E0-F040-9CD6-27D563352E45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9CCDBE04-1331-2A40-9C3A-F2E5E74B60BB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{9CCDBE04-1331-2A40-9C3A-F2E5E74B60BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Wage info</t>
   </si>
@@ -229,6 +229,15 @@
   </si>
   <si>
     <t>health_care benefits</t>
+  </si>
+  <si>
+    <t>medi_cal , dental vision</t>
+  </si>
+  <si>
+    <t>medi_cal , dental and vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medi_cal / dental / vision / life_insurance </t>
   </si>
 </sst>
 </file>
@@ -624,7 +633,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,6 +665,7 @@
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
         <v>14</v>
@@ -668,6 +678,7 @@
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -679,7 +690,7 @@
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="3"/>
@@ -694,7 +705,7 @@
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3"/>
@@ -707,6 +718,7 @@
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
         <v>6</v>
@@ -720,7 +732,7 @@
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3"/>
@@ -736,11 +748,12 @@
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="1"/>
@@ -749,11 +762,12 @@
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="1"/>
@@ -763,6 +777,7 @@
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
         <v>6</v>
@@ -776,16 +791,20 @@
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>14</v>
@@ -797,17 +816,21 @@
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
         <v>6</v>
@@ -821,6 +844,7 @@
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
@@ -834,6 +858,7 @@
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>14</v>
@@ -847,6 +872,7 @@
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
@@ -860,7 +886,7 @@
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -874,7 +900,7 @@
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -888,7 +914,7 @@
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="3"/>
@@ -900,7 +926,7 @@
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="3"/>
@@ -912,13 +938,14 @@
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="1"/>
@@ -927,6 +954,7 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>14</v>
@@ -940,23 +968,27 @@
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E24" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -964,7 +996,7 @@
       <c r="A26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="3"/>
@@ -979,7 +1011,7 @@
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -994,11 +1026,12 @@
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1006,6 +1039,7 @@
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1014,6 +1048,7 @@
       <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
         <v>6</v>
@@ -1026,6 +1061,7 @@
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="4" t="s">
         <v>23</v>
       </c>
@@ -1036,6 +1072,7 @@
       <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
         <v>6</v>
@@ -1046,6 +1083,7 @@
       <c r="A33" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>6</v>
@@ -1056,6 +1094,7 @@
       <c r="A34" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
         <v>6</v>

</xml_diff>